<commit_message>
added explanation in 데이터 worksheet
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="시간표" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="78">
   <si>
     <t>8:50~9:40</t>
   </si>
@@ -232,6 +232,46 @@
   </si>
   <si>
     <t>탐301</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>교과명</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>링크</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Link</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>교원</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>교실</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;- 위에서 교실 입력하면 자동으로 생성됨</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;- Zoom, Google Meet 밑에 링크를 넣으면 생성됨</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 워크시트의 데이터로 시간표가 만들어집니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://ksatimetable.herokuapp.com</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>버그, 문의사항 등은 20-017 김병권에게 연락해주시기 바랍니다.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -239,7 +279,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,6 +324,23 @@
       <name val="함초롬돋움"/>
       <family val="1"/>
       <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -348,7 +405,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -371,12 +428,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -435,11 +529,29 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -447,6 +559,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000FF"/>
+      <color rgb="FFFFA0A0"/>
+      <color rgb="FF00FFFF"/>
+      <color rgb="FF72E3F6"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -744,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -775,10 +895,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1"/>
@@ -808,8 +928,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="1"/>
       <c r="D3" s="6" t="str">
         <f>IF(ISBLANK(데이터!E6),IF(ISBLANK(데이터!F6),"",HYPERLINK(데이터!F6, 데이터!F1)),HYPERLINK(데이터!E6, 데이터!E1))</f>
@@ -829,10 +949,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="22" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1"/>
@@ -862,8 +982,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="1"/>
       <c r="D5" s="7" t="str">
         <f>IF(ISBLANK(데이터!E2),IF(ISBLANK(데이터!F2),"",HYPERLINK(데이터!F2, 데이터!F1)),HYPERLINK(데이터!E2, 데이터!E1))</f>
@@ -883,10 +1003,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="22" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="str">
@@ -911,8 +1031,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="7" t="str">
         <f>IF(ISBLANK(데이터!E2),IF(ISBLANK(데이터!F2),"",HYPERLINK(데이터!F2, 데이터!F1)),HYPERLINK(데이터!E2, 데이터!E1))</f>
         <v/>
@@ -929,10 +1049,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="3" t="str">
@@ -962,8 +1082,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="7" t="str">
         <f>IF(ISBLANK(데이터!E2),IF(ISBLANK(데이터!F2),"",HYPERLINK(데이터!F2, 데이터!F1)),HYPERLINK(데이터!E2, 데이터!E1))</f>
         <v/>
@@ -983,21 +1103,21 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
     </row>
     <row r="11" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="22" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="4" t="str">
@@ -1027,8 +1147,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="8" t="str">
         <f>IF(ISBLANK(데이터!E3),IF(ISBLANK(데이터!F3),"",HYPERLINK(데이터!F3, 데이터!F1)),HYPERLINK(데이터!E3, 데이터!E1))</f>
         <v/>
@@ -1048,10 +1168,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="5" t="str">
@@ -1086,8 +1206,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="9" t="str">
         <f>IF(ISBLANK(데이터!E4),IF(ISBLANK(데이터!F4),"",HYPERLINK(데이터!F4, 데이터!F1)),HYPERLINK(데이터!E4, 데이터!E1))</f>
         <v>Google Meet</v>
@@ -1110,10 +1230,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="22" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="15" t="str">
@@ -1133,8 +1253,8 @@
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="17" t="str">
         <f>IF(ISBLANK(데이터!E10),IF(ISBLANK(데이터!F10),"",HYPERLINK(데이터!F10, 데이터!F11)),HYPERLINK(데이터!E10, 데이터!E11))</f>
         <v/>
@@ -1148,10 +1268,10 @@
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="22" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="15" t="str">
@@ -1166,8 +1286,8 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="17" t="str">
         <f>IF(ISBLANK(데이터!E10),IF(ISBLANK(데이터!F10),"",HYPERLINK(데이터!F10, 데이터!F11)),HYPERLINK(데이터!E10, 데이터!E11))</f>
         <v/>
@@ -1178,10 +1298,10 @@
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="1"/>
@@ -1191,8 +1311,8 @@
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1200,21 +1320,21 @@
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
     </row>
     <row r="22" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="22" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="1"/>
@@ -1224,8 +1344,8 @@
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1233,10 +1353,10 @@
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="1"/>
@@ -1246,8 +1366,8 @@
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="20"/>
-      <c r="B25" s="20"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1256,6 +1376,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="A24:A25"/>
@@ -1268,18 +1400,6 @@
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1288,15 +1408,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="7" max="7" width="15.69921875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -1316,11 +1439,11 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>53</v>
       </c>
       <c r="C2" t="s">
@@ -1329,14 +1452,14 @@
       <c r="D2" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>54</v>
       </c>
       <c r="C3" t="s">
@@ -1345,14 +1468,14 @@
       <c r="D3" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>55</v>
       </c>
       <c r="C4" t="s">
@@ -1361,16 +1484,16 @@
       <c r="D4" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="22" t="s">
+      <c r="E4" s="20"/>
+      <c r="F4" s="21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>57</v>
       </c>
       <c r="C5" t="s">
@@ -1379,16 +1502,16 @@
       <c r="D5" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="21"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F5" s="20"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>59</v>
       </c>
       <c r="C6" t="s">
@@ -1397,16 +1520,16 @@
       <c r="D6" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="21"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F6" s="20"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>61</v>
       </c>
       <c r="C7" t="s">
@@ -1415,16 +1538,16 @@
       <c r="D7" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="21"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F7" s="20"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>63</v>
       </c>
       <c r="C8" t="s">
@@ -1433,16 +1556,16 @@
       <c r="D8" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="F8" s="21"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F8" s="20"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="20" t="s">
         <v>65</v>
       </c>
       <c r="C9" t="s">
@@ -1451,16 +1574,16 @@
       <c r="D9" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="21"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F9" s="20"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="20" t="s">
         <v>67</v>
       </c>
       <c r="C10" t="s">
@@ -1469,8 +1592,51 @@
       <c r="D10" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+    </row>
+    <row r="11" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G11" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G12" s="26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G13" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G14" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="H16" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="J16" s="28"/>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.4">
+      <c r="H17" s="30" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1481,7 +1647,9 @@
     <hyperlink ref="E9" r:id="rId4"/>
     <hyperlink ref="E5" r:id="rId5"/>
     <hyperlink ref="E8" r:id="rId6"/>
+    <hyperlink ref="I16" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>